<commit_message>
Added in derby database to program
</commit_message>
<xml_diff>
--- a/Inventory_Management/Avraam/savedInventory_Frozen.xlsx
+++ b/Inventory_Management/Avraam/savedInventory_Frozen.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="23" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
   <si>
     <t>Description</t>
   </si>
@@ -59,19 +59,10 @@
     <t>currentNumberOfItemsOnShelf</t>
   </si>
   <si>
-    <t>adasfsfa</t>
+    <t>Food</t>
   </si>
   <si>
     <t>F</t>
-  </si>
-  <si>
-    <t>asfuasfgufd</t>
-  </si>
-  <si>
-    <t>dsgegthjtrhkil7</t>
-  </si>
-  <si>
-    <t>grfefsdgtwq</t>
   </si>
 </sst>
 </file>
@@ -116,13 +107,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O5"/>
+  <dimension ref="A1:O2"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.0"/>
   <cols>
-    <col min="1" max="1" width="14.421875" customWidth="true" bestFit="true"/>
+    <col min="1" max="1" width="11.26171875" customWidth="true" bestFit="true"/>
     <col min="2" max="2" width="10.95703125" customWidth="true" bestFit="true"/>
     <col min="3" max="3" width="12.7109375" customWidth="true" bestFit="true"/>
     <col min="4" max="4" width="22.9296875" customWidth="true" bestFit="true"/>
@@ -203,115 +194,22 @@
         <v>1.0</v>
       </c>
       <c r="J2" t="n" s="0">
-        <v>10.0</v>
+        <v>100.0</v>
       </c>
       <c r="K2" t="n" s="0">
         <v>10.0</v>
       </c>
       <c r="L2" t="n" s="0">
-        <v>0.0</v>
+        <v>10.0</v>
       </c>
       <c r="M2" t="n" s="0">
-        <v>0.0</v>
+        <v>1.0</v>
       </c>
       <c r="N2" t="n" s="0">
         <v>0.0</v>
       </c>
       <c r="O2" t="n" s="0">
         <v>0.0</v>
-      </c>
-    </row>
-    <row r="3">
-      <c r="A3" t="s" s="0">
-        <v>17</v>
-      </c>
-      <c r="B3" t="n" s="0">
-        <v>1234.0</v>
-      </c>
-      <c r="C3" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D3" t="n" s="0">
-        <v>9.0</v>
-      </c>
-      <c r="E3" t="n" s="0">
-        <v>9.0</v>
-      </c>
-      <c r="J3" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="K3" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="L3" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="M3" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="N3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="O3" t="n" s="0">
-        <v>0.0</v>
-      </c>
-    </row>
-    <row r="4">
-      <c r="A4" t="s" s="0">
-        <v>18</v>
-      </c>
-      <c r="B4" t="n" s="0">
-        <v>123412.0</v>
-      </c>
-      <c r="C4" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="E4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="F4" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="G4" t="n" s="0">
-        <v>5.0</v>
-      </c>
-      <c r="H4" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="I4" t="n" s="0">
-        <v>10.0</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" t="s" s="0">
-        <v>19</v>
-      </c>
-      <c r="B5" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="C5" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D5" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="E5" t="n" s="0">
-        <v>2.0</v>
-      </c>
-      <c r="F5" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="G5" t="n" s="0">
-        <v>30.0</v>
-      </c>
-      <c r="H5" t="n" s="0">
-        <v>20.0</v>
-      </c>
-      <c r="I5" t="n" s="0">
-        <v>20.0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated GUI for Inventory
</commit_message>
<xml_diff>
--- a/Inventory_Management/Avraam/savedInventory_Frozen.xlsx
+++ b/Inventory_Management/Avraam/savedInventory_Frozen.xlsx
@@ -12,7 +12,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="17" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="15" uniqueCount="15">
   <si>
     <t>Description</t>
   </si>
@@ -58,12 +58,6 @@
   <si>
     <t>currentNumberOfItemsOnShelf</t>
   </si>
-  <si>
-    <t>Food</t>
-  </si>
-  <si>
-    <t>F</t>
-  </si>
 </sst>
 </file>
 
@@ -107,7 +101,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:O2"/>
+  <dimension ref="A1:O1"/>
   <sheetViews>
     <sheetView workbookViewId="0" tabSelected="true"/>
   </sheetViews>
@@ -177,41 +171,6 @@
         <v>14</v>
       </c>
     </row>
-    <row r="2">
-      <c r="A2" t="s" s="0">
-        <v>15</v>
-      </c>
-      <c r="B2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="C2" t="s" s="0">
-        <v>16</v>
-      </c>
-      <c r="D2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="E2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="J2" t="n" s="0">
-        <v>100.0</v>
-      </c>
-      <c r="K2" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="L2" t="n" s="0">
-        <v>10.0</v>
-      </c>
-      <c r="M2" t="n" s="0">
-        <v>1.0</v>
-      </c>
-      <c r="N2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-      <c r="O2" t="n" s="0">
-        <v>0.0</v>
-      </c>
-    </row>
   </sheetData>
   <pageMargins bottom="0.75" footer="0.3" header="0.3" left="0.7" right="0.7" top="0.75"/>
 </worksheet>

</xml_diff>